<commit_message>
Performed additional feature selection tests and added precision and f1 scores to most prediction results.
</commit_message>
<xml_diff>
--- a/Jeremy Thesis/Forecasting/January TS 5050 T1 Month Forecast Results.xlsx
+++ b/Jeremy Thesis/Forecasting/January TS 5050 T1 Month Forecast Results.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miste\PycharmProjects\SCAL_USIgnite-911\Jeremy Thesis\Forecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B429C1D-C4DE-4B23-95D0-00440F620062}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA802BC-EA06-4CB8-8072-15F1CFBB1926}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0F0AAEC9-2E63-408E-AAE1-6C90D48F886E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$49</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -23,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="61">
   <si>
     <t>TP</t>
   </si>
@@ -196,6 +201,24 @@
   </si>
   <si>
     <t>TS 5050 T1 1-31-2020</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>F1 Score</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>FS</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -266,13 +289,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -587,1150 +613,1741 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0F7AA82-2B71-4A71-8617-D396833D1986}">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="J1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>43838</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2">
+      <c r="D2" s="2">
         <v>53</v>
       </c>
-      <c r="C2" s="2">
+      <c r="E2" s="2">
         <v>40</v>
       </c>
-      <c r="D2" s="2">
+      <c r="F2" s="2">
         <v>4010</v>
       </c>
-      <c r="E2" s="2">
+      <c r="G2" s="2">
         <v>496</v>
       </c>
-      <c r="F2" s="3">
+      <c r="H2" s="3">
         <v>0.56989247311827895</v>
       </c>
-      <c r="G2" s="3">
+      <c r="I2" s="3">
         <v>0.88992454505104301</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="J2" s="3">
+        <v>9.6539162112932608</v>
+      </c>
+      <c r="K2" s="3">
+        <v>16.510903426791277</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>43838</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="4">
+      <c r="D3" s="4">
         <v>36</v>
       </c>
-      <c r="C3" s="4">
+      <c r="E3" s="4">
         <v>56</v>
       </c>
-      <c r="D3" s="4">
+      <c r="F3" s="4">
         <v>3730</v>
       </c>
-      <c r="E3" s="4">
+      <c r="G3" s="4">
         <v>651</v>
       </c>
-      <c r="F3" s="5">
+      <c r="H3" s="5">
         <v>0.39130434782608697</v>
       </c>
-      <c r="G3" s="5">
+      <c r="I3" s="5">
         <v>0.85140378908924896</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="J3" s="5">
+        <v>5.2401746724890828</v>
+      </c>
+      <c r="K3" s="5">
+        <v>9.2426187419768926</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>43839</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2">
+      <c r="D4" s="2">
         <v>53</v>
       </c>
-      <c r="C4" s="2">
+      <c r="E4" s="2">
         <v>32</v>
       </c>
-      <c r="D4" s="2">
+      <c r="F4" s="2">
         <v>3665</v>
       </c>
-      <c r="E4" s="2">
+      <c r="G4" s="2">
         <v>849</v>
       </c>
-      <c r="F4" s="3">
+      <c r="H4" s="3">
         <v>0.623529411764705</v>
       </c>
-      <c r="G4" s="3">
+      <c r="I4" s="3">
         <v>0.811918475852902</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="J4" s="3">
+        <v>5.8758314855875833</v>
+      </c>
+      <c r="K4" s="3">
+        <v>10.739614994934144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>43839</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="4">
+      <c r="D5" s="4">
         <v>24</v>
       </c>
-      <c r="C5" s="4">
-        <v>59</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="E5" s="4">
+        <v>59</v>
+      </c>
+      <c r="F5" s="4">
         <v>3737</v>
       </c>
-      <c r="E5" s="4">
+      <c r="G5" s="4">
         <v>653</v>
       </c>
-      <c r="F5" s="5">
+      <c r="H5" s="5">
         <v>0.28915662650602397</v>
       </c>
-      <c r="G5" s="5">
+      <c r="I5" s="5">
         <v>0.85125284738040996</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="J5" s="5">
+        <v>3.5450516986706058</v>
+      </c>
+      <c r="K5" s="5">
+        <v>6.3157894736842106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>43840</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2">
+      <c r="D6" s="2">
         <v>46</v>
       </c>
-      <c r="C6" s="2">
+      <c r="E6" s="2">
         <v>26</v>
       </c>
-      <c r="D6" s="2">
+      <c r="F6" s="2">
         <v>3878</v>
       </c>
-      <c r="E6" s="2">
+      <c r="G6" s="2">
         <v>649</v>
       </c>
-      <c r="F6" s="3">
+      <c r="H6" s="3">
         <v>0.63888888888888795</v>
       </c>
-      <c r="G6" s="3">
+      <c r="I6" s="3">
         <v>0.85663795007731303</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="J6" s="3">
+        <v>6.6187050359712227</v>
+      </c>
+      <c r="K6" s="3">
+        <v>11.994784876140809</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>43840</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="4">
+      <c r="D7" s="4">
         <v>27</v>
       </c>
-      <c r="C7" s="4">
+      <c r="E7" s="4">
         <v>41</v>
       </c>
-      <c r="D7" s="4">
+      <c r="F7" s="4">
         <v>3459</v>
       </c>
-      <c r="E7" s="4">
+      <c r="G7" s="4">
         <v>946</v>
       </c>
-      <c r="F7" s="5">
+      <c r="H7" s="5">
         <v>0.39705882352941102</v>
       </c>
-      <c r="G7" s="5">
+      <c r="I7" s="5">
         <v>0.78524404086265598</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="J7" s="5">
+        <v>2.7749229188078108</v>
+      </c>
+      <c r="K7" s="5">
+        <v>5.1873198847262243</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>43841</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="2">
+      <c r="D8" s="2">
         <v>64</v>
       </c>
-      <c r="C8" s="2">
+      <c r="E8" s="2">
         <v>45</v>
       </c>
-      <c r="D8" s="2">
+      <c r="F8" s="2">
         <v>3761</v>
       </c>
-      <c r="E8" s="2">
+      <c r="G8" s="2">
         <v>729</v>
       </c>
-      <c r="F8" s="3">
+      <c r="H8" s="3">
         <v>0.58715596330275199</v>
       </c>
-      <c r="G8" s="3">
+      <c r="I8" s="3">
         <v>0.83763919821826205</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="J8" s="3">
+        <v>8.0706179066834807</v>
+      </c>
+      <c r="K8" s="3">
+        <v>14.190687361419069</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>43841</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="4">
+      <c r="D9" s="4">
         <v>53</v>
       </c>
-      <c r="C9" s="4">
+      <c r="E9" s="4">
         <v>56</v>
       </c>
-      <c r="D9" s="4">
+      <c r="F9" s="4">
         <v>3541</v>
       </c>
-      <c r="E9" s="4">
+      <c r="G9" s="4">
         <v>823</v>
       </c>
-      <c r="F9" s="5">
+      <c r="H9" s="5">
         <v>0.48623853211009099</v>
       </c>
-      <c r="G9" s="5">
+      <c r="I9" s="5">
         <v>0.81141154903757995</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="J9" s="5">
+        <v>6.0502283105022832</v>
+      </c>
+      <c r="K9" s="5">
+        <v>10.761421319796952</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>43842</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2">
+      <c r="D10" s="2">
         <v>62</v>
       </c>
-      <c r="C10" s="2">
+      <c r="E10" s="2">
         <v>56</v>
       </c>
-      <c r="D10" s="2">
+      <c r="F10" s="2">
         <v>3971</v>
       </c>
-      <c r="E10" s="2">
+      <c r="G10" s="2">
         <v>510</v>
       </c>
-      <c r="F10" s="3">
+      <c r="H10" s="3">
         <v>0.52542372881355903</v>
       </c>
-      <c r="G10" s="3">
+      <c r="I10" s="3">
         <v>0.88618611916982803</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="J10" s="3">
+        <v>10.839160839160838</v>
+      </c>
+      <c r="K10" s="3">
+        <v>17.971014492753625</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>43842</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="4">
+      <c r="D11" s="4">
         <v>51</v>
       </c>
-      <c r="C11" s="4">
+      <c r="E11" s="4">
         <v>67</v>
       </c>
-      <c r="D11" s="4">
+      <c r="F11" s="4">
         <v>3709</v>
       </c>
-      <c r="E11" s="4">
+      <c r="G11" s="4">
         <v>646</v>
       </c>
-      <c r="F11" s="5">
+      <c r="H11" s="5">
         <v>0.43220338983050799</v>
       </c>
-      <c r="G11" s="5">
+      <c r="I11" s="5">
         <v>0.85166475315728996</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="J11" s="5">
+        <v>7.3170731707317067</v>
+      </c>
+      <c r="K11" s="5">
+        <v>12.515337423312884</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>43843</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2">
+      <c r="D12" s="2">
         <v>45</v>
       </c>
-      <c r="C12" s="2">
+      <c r="E12" s="2">
         <v>69</v>
       </c>
-      <c r="D12" s="2">
+      <c r="F12" s="2">
         <v>3774</v>
       </c>
-      <c r="E12" s="2">
+      <c r="G12" s="2">
         <v>711</v>
       </c>
-      <c r="F12" s="3">
+      <c r="H12" s="3">
         <v>0.394736842105263</v>
       </c>
-      <c r="G12" s="3">
+      <c r="I12" s="3">
         <v>0.84147157190635402</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="J12" s="3">
+        <v>5.9523809523809517</v>
+      </c>
+      <c r="K12" s="3">
+        <v>10.344827586206895</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>43843</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="4">
+      <c r="D13" s="4">
         <v>25</v>
       </c>
-      <c r="C13" s="4">
+      <c r="E13" s="4">
         <v>85</v>
       </c>
-      <c r="D13" s="4">
+      <c r="F13" s="4">
         <v>3675</v>
       </c>
-      <c r="E13" s="4">
+      <c r="G13" s="4">
         <v>688</v>
       </c>
-      <c r="F13" s="5">
+      <c r="H13" s="5">
         <v>0.22727272727272699</v>
       </c>
-      <c r="G13" s="5">
+      <c r="I13" s="5">
         <v>0.84231033692413404</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="J13" s="5">
+        <v>3.5063113604488079</v>
+      </c>
+      <c r="K13" s="5">
+        <v>6.0753341433778845</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>43844</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="2">
+      <c r="D14" s="2">
         <v>75</v>
       </c>
-      <c r="C14" s="2">
+      <c r="E14" s="2">
         <v>24</v>
       </c>
-      <c r="D14" s="2">
+      <c r="F14" s="2">
         <v>3715</v>
       </c>
-      <c r="E14" s="2">
+      <c r="G14" s="2">
         <v>785</v>
       </c>
-      <c r="F14" s="3">
+      <c r="H14" s="3">
         <v>0.75757575757575701</v>
       </c>
-      <c r="G14" s="3">
+      <c r="I14" s="3">
         <v>0.82555555555555504</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="J14" s="3">
+        <v>8.720930232558139</v>
+      </c>
+      <c r="K14" s="3">
+        <v>15.641293013555787</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>43844</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="4">
+      <c r="D15" s="4">
         <v>46</v>
       </c>
-      <c r="C15" s="4">
+      <c r="E15" s="4">
         <v>52</v>
       </c>
-      <c r="D15" s="4">
+      <c r="F15" s="4">
         <v>3329</v>
       </c>
-      <c r="E15" s="4">
+      <c r="G15" s="4">
         <v>1046</v>
       </c>
-      <c r="F15" s="5">
+      <c r="H15" s="5">
         <v>0.46938775510204001</v>
       </c>
-      <c r="G15" s="5">
+      <c r="I15" s="5">
         <v>0.76091428571428499</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="J15" s="5">
+        <v>4.2124542124542126</v>
+      </c>
+      <c r="K15" s="5">
+        <v>7.73109243697479</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>43845</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="2">
+      <c r="D16" s="2">
         <v>49</v>
       </c>
-      <c r="C16" s="2">
+      <c r="E16" s="2">
         <v>38</v>
       </c>
-      <c r="D16" s="2">
+      <c r="F16" s="2">
         <v>3868</v>
       </c>
-      <c r="E16" s="2">
+      <c r="G16" s="2">
         <v>644</v>
       </c>
-      <c r="F16" s="3">
+      <c r="H16" s="3">
         <v>0.56321839080459701</v>
       </c>
-      <c r="G16" s="3">
+      <c r="I16" s="3">
         <v>0.85726950354609899</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="J16" s="3">
+        <v>7.0707070707070701</v>
+      </c>
+      <c r="K16" s="3">
+        <v>12.56410256410256</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>43845</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="4">
+      <c r="D17" s="4">
         <v>27</v>
       </c>
-      <c r="C17" s="4">
-        <v>59</v>
-      </c>
-      <c r="D17" s="4">
+      <c r="E17" s="4">
+        <v>59</v>
+      </c>
+      <c r="F17" s="4">
         <v>3466</v>
       </c>
-      <c r="E17" s="4">
+      <c r="G17" s="4">
         <v>921</v>
       </c>
-      <c r="F17" s="5">
+      <c r="H17" s="5">
         <v>0.31395348837209303</v>
       </c>
-      <c r="G17" s="5">
+      <c r="I17" s="5">
         <v>0.79006154547526697</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="J17" s="5">
+        <v>2.8481012658227849</v>
+      </c>
+      <c r="K17" s="5">
+        <v>5.222437137330755</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>43846</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="2">
+      <c r="D18" s="2">
         <v>46</v>
       </c>
-      <c r="C18" s="2">
+      <c r="E18" s="2">
         <v>15</v>
       </c>
-      <c r="D18" s="2">
+      <c r="F18" s="2">
         <v>3973</v>
       </c>
-      <c r="E18" s="2">
+      <c r="G18" s="2">
         <v>565</v>
       </c>
-      <c r="F18" s="3">
+      <c r="H18" s="3">
         <v>0.75409836065573699</v>
       </c>
-      <c r="G18" s="3">
+      <c r="I18" s="3">
         <v>0.87549581313353897</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="J18" s="3">
+        <v>7.5286415711947621</v>
+      </c>
+      <c r="K18" s="3">
+        <v>13.69047619047619</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>43846</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="4">
+      <c r="D19" s="4">
         <v>14</v>
       </c>
-      <c r="C19" s="4">
+      <c r="E19" s="4">
         <v>47</v>
       </c>
-      <c r="D19" s="4">
+      <c r="F19" s="4">
         <v>3957</v>
       </c>
-      <c r="E19" s="4">
+      <c r="G19" s="4">
         <v>455</v>
       </c>
-      <c r="F19" s="5">
+      <c r="H19" s="5">
         <v>0.22950819672131101</v>
       </c>
-      <c r="G19" s="5">
+      <c r="I19" s="5">
         <v>0.89687216681776905</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="J19" s="5">
+        <v>2.9850746268656714</v>
+      </c>
+      <c r="K19" s="5">
+        <v>5.2830188679245271</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>43847</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="2">
+      <c r="D20" s="2">
         <v>53</v>
       </c>
-      <c r="C20" s="2">
+      <c r="E20" s="2">
         <v>31</v>
       </c>
-      <c r="D20" s="2">
+      <c r="F20" s="2">
         <v>3810</v>
       </c>
-      <c r="E20" s="2">
+      <c r="G20" s="2">
         <v>705</v>
       </c>
-      <c r="F20" s="3">
+      <c r="H20" s="3">
         <v>0.63095238095238004</v>
       </c>
-      <c r="G20" s="3">
+      <c r="I20" s="3">
         <v>0.84385382059800595</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="J20" s="3">
+        <v>6.9920844327176779</v>
+      </c>
+      <c r="K20" s="3">
+        <v>12.589073634204272</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>43847</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="4">
+      <c r="D21" s="4">
         <v>25</v>
       </c>
-      <c r="C21" s="4">
+      <c r="E21" s="4">
         <v>57</v>
       </c>
-      <c r="D21" s="4">
+      <c r="F21" s="4">
         <v>3610</v>
       </c>
-      <c r="E21" s="4">
+      <c r="G21" s="4">
         <v>781</v>
       </c>
-      <c r="F21" s="5">
+      <c r="H21" s="5">
         <v>0.30487804878048702</v>
       </c>
-      <c r="G21" s="5">
+      <c r="I21" s="5">
         <v>0.82213618765657004</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="J21" s="5">
+        <v>3.1017369727047148</v>
+      </c>
+      <c r="K21" s="5">
+        <v>5.6306306306306295</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <v>43848</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="2">
+      <c r="D22" s="2">
         <v>84</v>
       </c>
-      <c r="C22" s="2">
+      <c r="E22" s="2">
         <v>75</v>
       </c>
-      <c r="D22" s="2">
+      <c r="F22" s="2">
         <v>3907</v>
       </c>
-      <c r="E22" s="2">
+      <c r="G22" s="2">
         <v>533</v>
       </c>
-      <c r="F22" s="3">
+      <c r="H22" s="3">
         <v>0.52830188679245205</v>
       </c>
-      <c r="G22" s="3">
+      <c r="I22" s="3">
         <v>0.87995495495495402</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="J22" s="3">
+        <v>13.614262560777956</v>
+      </c>
+      <c r="K22" s="3">
+        <v>21.649484536082468</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>43848</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="4">
-        <v>59</v>
-      </c>
-      <c r="C23" s="4">
+      <c r="D23" s="4">
+        <v>59</v>
+      </c>
+      <c r="E23" s="4">
         <v>96</v>
       </c>
-      <c r="D23" s="4">
+      <c r="F23" s="4">
         <v>3622</v>
       </c>
-      <c r="E23" s="4">
+      <c r="G23" s="4">
         <v>696</v>
       </c>
-      <c r="F23" s="5">
+      <c r="H23" s="5">
         <v>0.380645161290322</v>
       </c>
-      <c r="G23" s="5">
+      <c r="I23" s="5">
         <v>0.83881426586382501</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="J23" s="5">
+        <v>7.8145695364238401</v>
+      </c>
+      <c r="K23" s="5">
+        <v>12.967032967032962</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <v>43849</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="2">
+      <c r="D24" s="2">
         <v>33</v>
       </c>
-      <c r="C24" s="2">
+      <c r="E24" s="2">
         <v>29</v>
       </c>
-      <c r="D24" s="2">
+      <c r="F24" s="2">
         <v>3788</v>
       </c>
-      <c r="E24" s="2">
+      <c r="G24" s="2">
         <v>749</v>
       </c>
-      <c r="F24" s="3">
+      <c r="H24" s="3">
         <v>0.532258064516129</v>
       </c>
-      <c r="G24" s="3">
+      <c r="I24" s="3">
         <v>0.83491293806480005</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="J24" s="3">
+        <v>4.2199488491048589</v>
+      </c>
+      <c r="K24" s="3">
+        <v>7.8199052132701423</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>43849</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="4">
+      <c r="D25" s="4">
         <v>25</v>
       </c>
-      <c r="C25" s="4">
+      <c r="E25" s="4">
         <v>37</v>
       </c>
-      <c r="D25" s="4">
+      <c r="F25" s="4">
         <v>3452</v>
       </c>
-      <c r="E25" s="4">
+      <c r="G25" s="4">
         <v>959</v>
       </c>
-      <c r="F25" s="5">
+      <c r="H25" s="5">
         <v>0.40322580645161199</v>
       </c>
-      <c r="G25" s="5">
+      <c r="I25" s="5">
         <v>0.78258898209022898</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="J25" s="5">
+        <v>2.5406504065040649</v>
+      </c>
+      <c r="K25" s="5">
+        <v>4.7801147227533463</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
+        <v>43850</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="2">
+      <c r="D26" s="2">
         <v>49</v>
       </c>
-      <c r="C26" s="2">
+      <c r="E26" s="2">
         <v>35</v>
       </c>
-      <c r="D26" s="2">
+      <c r="F26" s="2">
         <v>4022</v>
       </c>
-      <c r="E26" s="2">
+      <c r="G26" s="2">
         <v>493</v>
       </c>
-      <c r="F26" s="3">
+      <c r="H26" s="3">
         <v>0.58333333333333304</v>
       </c>
-      <c r="G26" s="3">
+      <c r="I26" s="3">
         <v>0.89080841638981101</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="J26" s="3">
+        <v>9.0405904059040587</v>
+      </c>
+      <c r="K26" s="3">
+        <v>15.654952076677315</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>43850</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="4">
+      <c r="D27" s="4">
         <v>11</v>
       </c>
-      <c r="C27" s="4">
+      <c r="E27" s="4">
         <v>71</v>
       </c>
-      <c r="D27" s="4">
+      <c r="F27" s="4">
         <v>3891</v>
       </c>
-      <c r="E27" s="4">
+      <c r="G27" s="4">
         <v>500</v>
       </c>
-      <c r="F27" s="5">
+      <c r="H27" s="5">
         <v>0.134146341463414</v>
       </c>
-      <c r="G27" s="5">
+      <c r="I27" s="5">
         <v>0.886130721931223</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="J27" s="5">
+        <v>2.152641878669276</v>
+      </c>
+      <c r="K27" s="5">
+        <v>3.7099494097807733</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="8">
+        <v>43851</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="2">
+      <c r="D28" s="2">
         <v>58</v>
       </c>
-      <c r="C28" s="2">
+      <c r="E28" s="2">
         <v>33</v>
       </c>
-      <c r="D28" s="2">
+      <c r="F28" s="2">
         <v>3841</v>
       </c>
-      <c r="E28" s="2">
+      <c r="G28" s="2">
         <v>667</v>
       </c>
-      <c r="F28" s="3">
+      <c r="H28" s="3">
         <v>0.63736263736263699</v>
       </c>
-      <c r="G28" s="3">
+      <c r="I28" s="3">
         <v>0.85204081632652995</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="J28" s="3">
+        <v>8</v>
+      </c>
+      <c r="K28" s="3">
+        <v>14.215686274509803</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>43851</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="4">
+      <c r="D29" s="4">
         <v>29</v>
       </c>
-      <c r="C29" s="4">
+      <c r="E29" s="4">
         <v>62</v>
       </c>
-      <c r="D29" s="4">
+      <c r="F29" s="4">
         <v>3914</v>
       </c>
-      <c r="E29" s="4">
+      <c r="G29" s="4">
         <v>468</v>
       </c>
-      <c r="F29" s="5">
+      <c r="H29" s="5">
         <v>0.31868131868131799</v>
       </c>
-      <c r="G29" s="5">
+      <c r="I29" s="5">
         <v>0.89319945230488296</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="J29" s="5">
+        <v>5.8350100603621735</v>
+      </c>
+      <c r="K29" s="5">
+        <v>9.8639455782312879</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="8">
+        <v>43852</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="2">
+      <c r="D30" s="2">
         <v>61</v>
       </c>
-      <c r="C30" s="2">
+      <c r="E30" s="2">
         <v>15</v>
       </c>
-      <c r="D30" s="2">
+      <c r="F30" s="2">
         <v>3631</v>
       </c>
-      <c r="E30" s="2">
+      <c r="G30" s="2">
         <v>892</v>
       </c>
-      <c r="F30" s="3">
+      <c r="H30" s="3">
         <v>0.80263157894736803</v>
       </c>
-      <c r="G30" s="3">
+      <c r="I30" s="3">
         <v>0.80278576166261295</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="J30" s="3">
+        <v>6.4008394543546689</v>
+      </c>
+      <c r="K30" s="3">
+        <v>11.856171039844508</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <v>43852</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="4">
+      <c r="D31" s="4">
         <v>26</v>
       </c>
-      <c r="C31" s="4">
+      <c r="E31" s="4">
         <v>49</v>
       </c>
-      <c r="D31" s="4">
+      <c r="F31" s="4">
         <v>3706</v>
       </c>
-      <c r="E31" s="4">
+      <c r="G31" s="4">
         <v>692</v>
       </c>
-      <c r="F31" s="5">
+      <c r="H31" s="5">
         <v>0.34666666666666601</v>
       </c>
-      <c r="G31" s="5">
+      <c r="I31" s="5">
         <v>0.84265575261482495</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="J31" s="5">
+        <v>3.6211699164345403</v>
+      </c>
+      <c r="K31" s="5">
+        <v>6.5573770491803272</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="8">
+        <v>43853</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B32" s="2">
+      <c r="D32" s="2">
         <v>84</v>
       </c>
-      <c r="C32" s="2">
+      <c r="E32" s="2">
         <v>46</v>
       </c>
-      <c r="D32" s="2">
+      <c r="F32" s="2">
         <v>3827</v>
       </c>
-      <c r="E32" s="2">
+      <c r="G32" s="2">
         <v>642</v>
       </c>
-      <c r="F32" s="3">
+      <c r="H32" s="3">
         <v>0.64615384615384597</v>
       </c>
-      <c r="G32" s="3">
+      <c r="I32" s="3">
         <v>0.856343701051689</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="J32" s="3">
+        <v>11.570247933884298</v>
+      </c>
+      <c r="K32" s="3">
+        <v>19.626168224299064</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <v>43853</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="4">
+      <c r="D33" s="4">
         <v>62</v>
       </c>
-      <c r="C33" s="4">
+      <c r="E33" s="4">
         <v>66</v>
       </c>
-      <c r="D33" s="4">
+      <c r="F33" s="4">
         <v>3487</v>
       </c>
-      <c r="E33" s="4">
+      <c r="G33" s="4">
         <v>858</v>
       </c>
-      <c r="F33" s="5">
+      <c r="H33" s="5">
         <v>0.484375</v>
       </c>
-      <c r="G33" s="5">
+      <c r="I33" s="5">
         <v>0.80253164556961998</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="J33" s="5">
+        <v>6.7391304347826084</v>
+      </c>
+      <c r="K33" s="5">
+        <v>11.83206106870229</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="8">
+        <v>43854</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="2">
+      <c r="D34" s="2">
         <v>69</v>
       </c>
-      <c r="C34" s="2">
+      <c r="E34" s="2">
         <v>45</v>
       </c>
-      <c r="D34" s="2">
+      <c r="F34" s="2">
         <v>3873</v>
       </c>
-      <c r="E34" s="2">
+      <c r="G34" s="2">
         <v>612</v>
       </c>
-      <c r="F34" s="3">
+      <c r="H34" s="3">
         <v>0.60526315789473595</v>
       </c>
-      <c r="G34" s="3">
+      <c r="I34" s="3">
         <v>0.86354515050167202</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="J34" s="3">
+        <v>10.13215859030837</v>
+      </c>
+      <c r="K34" s="3">
+        <v>17.35849056603773</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <v>43854</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="4">
+      <c r="D35" s="4">
         <v>24</v>
       </c>
-      <c r="C35" s="4">
+      <c r="E35" s="4">
         <v>89</v>
       </c>
-      <c r="D35" s="4">
+      <c r="F35" s="4">
         <v>3663</v>
       </c>
-      <c r="E35" s="4">
+      <c r="G35" s="4">
         <v>697</v>
       </c>
-      <c r="F35" s="5">
+      <c r="H35" s="5">
         <v>0.212389380530973</v>
       </c>
-      <c r="G35" s="5">
+      <c r="I35" s="5">
         <v>0.84013761467889903</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="J35" s="5">
+        <v>3.3287101248266295</v>
+      </c>
+      <c r="K35" s="5">
+        <v>5.7553956834532354</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="8">
+        <v>43855</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="2">
+      <c r="D36" s="2">
         <v>43</v>
       </c>
-      <c r="C36" s="2">
+      <c r="E36" s="2">
         <v>28</v>
       </c>
-      <c r="D36" s="2">
+      <c r="F36" s="2">
         <v>3859</v>
       </c>
-      <c r="E36" s="2">
+      <c r="G36" s="2">
         <v>669</v>
       </c>
-      <c r="F36" s="3">
+      <c r="H36" s="3">
         <v>0.60563380281690105</v>
       </c>
-      <c r="G36" s="3">
+      <c r="I36" s="3">
         <v>0.85225265017667795</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="J36" s="3">
+        <v>6.0393258426966296</v>
+      </c>
+      <c r="K36" s="3">
+        <v>10.983397190293742</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
+        <v>43855</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B37" s="4">
+      <c r="D37" s="4">
         <v>22</v>
       </c>
-      <c r="C37" s="4">
+      <c r="E37" s="4">
         <v>49</v>
       </c>
-      <c r="D37" s="4">
+      <c r="F37" s="4">
         <v>3339</v>
       </c>
-      <c r="E37" s="4">
+      <c r="G37" s="4">
         <v>1063</v>
       </c>
-      <c r="F37" s="5">
+      <c r="H37" s="5">
         <v>0.309859154929577</v>
       </c>
-      <c r="G37" s="5">
+      <c r="I37" s="5">
         <v>0.75851885506587902</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="J37" s="5">
+        <v>2.0276497695852536</v>
+      </c>
+      <c r="K37" s="5">
+        <v>3.8062283737024223</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="8">
+        <v>43856</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="2">
+      <c r="D38" s="2">
         <v>25</v>
       </c>
-      <c r="C38" s="2">
+      <c r="E38" s="2">
         <v>31</v>
       </c>
-      <c r="D38" s="2">
+      <c r="F38" s="2">
         <v>3822</v>
       </c>
-      <c r="E38" s="2">
+      <c r="G38" s="2">
         <v>721</v>
       </c>
-      <c r="F38" s="3">
+      <c r="H38" s="3">
         <v>0.44642857142857101</v>
       </c>
-      <c r="G38" s="3">
+      <c r="I38" s="3">
         <v>0.84129429892141705</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+      <c r="J38" s="3">
+        <v>3.3512064343163539</v>
+      </c>
+      <c r="K38" s="3">
+        <v>6.2344139650872812</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
+        <v>43856</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B39" s="4">
+      <c r="D39" s="4">
         <v>9</v>
       </c>
-      <c r="C39" s="4">
+      <c r="E39" s="4">
         <v>47</v>
       </c>
-      <c r="D39" s="4">
+      <c r="F39" s="4">
         <v>3655</v>
       </c>
-      <c r="E39" s="4">
+      <c r="G39" s="4">
         <v>762</v>
       </c>
-      <c r="F39" s="5">
+      <c r="H39" s="5">
         <v>0.160714285714285</v>
       </c>
-      <c r="G39" s="5">
+      <c r="I39" s="5">
         <v>0.82748471813447999</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="J39" s="5">
+        <v>1.1673151750972763</v>
+      </c>
+      <c r="K39" s="5">
+        <v>2.1765417170495764</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="8">
+        <v>43857</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="2">
+      <c r="D40" s="2">
         <v>63</v>
       </c>
-      <c r="C40" s="2">
+      <c r="E40" s="2">
         <v>43</v>
       </c>
-      <c r="D40" s="2">
+      <c r="F40" s="2">
         <v>3868</v>
       </c>
-      <c r="E40" s="2">
+      <c r="G40" s="2">
         <v>625</v>
       </c>
-      <c r="F40" s="3">
+      <c r="H40" s="3">
         <v>0.59433962264150897</v>
       </c>
-      <c r="G40" s="3">
+      <c r="I40" s="3">
         <v>0.86089472512797605</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
+      <c r="J40" s="3">
+        <v>9.1569767441860463</v>
+      </c>
+      <c r="K40" s="3">
+        <v>15.86901763224181</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
+        <v>43857</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B41" s="4">
+      <c r="D41" s="4">
         <v>35</v>
       </c>
-      <c r="C41" s="4">
+      <c r="E41" s="4">
         <v>70</v>
       </c>
-      <c r="D41" s="4">
+      <c r="F41" s="4">
         <v>3506</v>
       </c>
-      <c r="E41" s="4">
+      <c r="G41" s="4">
         <v>862</v>
       </c>
-      <c r="F41" s="5">
+      <c r="H41" s="5">
         <v>0.33333333333333298</v>
       </c>
-      <c r="G41" s="5">
+      <c r="I41" s="5">
         <v>0.80265567765567702</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="J41" s="5">
+        <v>3.9018952062430321</v>
+      </c>
+      <c r="K41" s="5">
+        <v>6.9860279441117754</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="8">
+        <v>43858</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B42" s="2">
+      <c r="D42" s="2">
         <v>37</v>
       </c>
-      <c r="C42" s="2">
+      <c r="E42" s="2">
         <v>31</v>
       </c>
-      <c r="D42" s="2">
+      <c r="F42" s="2">
         <v>3963</v>
       </c>
-      <c r="E42" s="2">
+      <c r="G42" s="2">
         <v>568</v>
       </c>
-      <c r="F42" s="3">
+      <c r="H42" s="3">
         <v>0.54411764705882304</v>
       </c>
-      <c r="G42" s="3">
+      <c r="I42" s="3">
         <v>0.87464135952328403</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+      <c r="J42" s="3">
+        <v>6.115702479338843</v>
+      </c>
+      <c r="K42" s="3">
+        <v>10.995542347696878</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
+        <v>43858</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B43" s="4">
+      <c r="D43" s="4">
         <v>20</v>
       </c>
-      <c r="C43" s="4">
+      <c r="E43" s="4">
         <v>48</v>
       </c>
-      <c r="D43" s="4">
+      <c r="F43" s="4">
         <v>3958</v>
       </c>
-      <c r="E43" s="4">
+      <c r="G43" s="4">
         <v>447</v>
       </c>
-      <c r="F43" s="5">
+      <c r="H43" s="5">
         <v>0.29411764705882298</v>
       </c>
-      <c r="G43" s="5">
+      <c r="I43" s="5">
         <v>0.89852440408626499</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="J43" s="5">
+        <v>4.2826552462526761</v>
+      </c>
+      <c r="K43" s="5">
+        <v>7.4766355140186898</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="8">
+        <v>43859</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B44" s="2">
+      <c r="D44" s="2">
         <v>54</v>
       </c>
-      <c r="C44" s="2">
+      <c r="E44" s="2">
         <v>27</v>
       </c>
-      <c r="D44" s="2">
+      <c r="F44" s="2">
         <v>3860</v>
       </c>
-      <c r="E44" s="2">
+      <c r="G44" s="2">
         <v>658</v>
       </c>
-      <c r="F44" s="3">
+      <c r="H44" s="3">
         <v>0.66666666666666596</v>
       </c>
-      <c r="G44" s="3">
+      <c r="I44" s="3">
         <v>0.85436033643204901</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+      <c r="J44" s="3">
+        <v>7.5842696629213489</v>
+      </c>
+      <c r="K44" s="3">
+        <v>13.619167717528372</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
+        <v>43859</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B45" s="4">
+      <c r="D45" s="4">
         <v>31</v>
       </c>
-      <c r="C45" s="4">
+      <c r="E45" s="4">
         <v>49</v>
       </c>
-      <c r="D45" s="4">
+      <c r="F45" s="4">
         <v>3605</v>
       </c>
-      <c r="E45" s="4">
+      <c r="G45" s="4">
         <v>788</v>
       </c>
-      <c r="F45" s="5">
+      <c r="H45" s="5">
         <v>0.38750000000000001</v>
       </c>
-      <c r="G45" s="5">
+      <c r="I45" s="5">
         <v>0.82062371955383495</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="J45" s="5">
+        <v>3.785103785103785</v>
+      </c>
+      <c r="K45" s="5">
+        <v>6.8965517241379306</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="8">
+        <v>43860</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B46" s="2">
+      <c r="D46" s="2">
         <v>29</v>
       </c>
-      <c r="C46" s="2">
+      <c r="E46" s="2">
         <v>23</v>
       </c>
-      <c r="D46" s="2">
+      <c r="F46" s="2">
         <v>4050</v>
       </c>
-      <c r="E46" s="2">
+      <c r="G46" s="2">
         <v>497</v>
       </c>
-      <c r="F46" s="3">
+      <c r="H46" s="3">
         <v>0.55769230769230704</v>
       </c>
-      <c r="G46" s="3">
+      <c r="I46" s="3">
         <v>0.890697162964592</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+      <c r="J46" s="3">
+        <v>5.5133079847908748</v>
+      </c>
+      <c r="K46" s="3">
+        <v>10.034602076124566</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="7">
+        <v>43860</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C47" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B47" s="4">
+      <c r="D47" s="4">
         <v>24</v>
       </c>
-      <c r="C47" s="4">
+      <c r="E47" s="4">
         <v>28</v>
       </c>
-      <c r="D47" s="4">
+      <c r="F47" s="4">
         <v>3628</v>
       </c>
-      <c r="E47" s="4">
+      <c r="G47" s="4">
         <v>793</v>
       </c>
-      <c r="F47" s="5">
+      <c r="H47" s="5">
         <v>0.46153846153846101</v>
       </c>
-      <c r="G47" s="5">
+      <c r="I47" s="5">
         <v>0.82062881700972601</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="J47" s="5">
+        <v>2.9375764993880051</v>
+      </c>
+      <c r="K47" s="5">
+        <v>5.5235903337169159</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="8">
+        <v>43861</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B48" s="2">
+      <c r="D48" s="2">
         <v>48</v>
       </c>
-      <c r="C48" s="2">
+      <c r="E48" s="2">
         <v>43</v>
       </c>
-      <c r="D48" s="2">
+      <c r="F48" s="2">
         <v>3701</v>
       </c>
-      <c r="E48" s="2">
+      <c r="G48" s="2">
         <v>807</v>
       </c>
-      <c r="F48" s="3">
+      <c r="H48" s="3">
         <v>0.52747252747252704</v>
       </c>
-      <c r="G48" s="3">
+      <c r="I48" s="3">
         <v>0.82098491570541199</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
+      <c r="J48" s="3">
+        <v>5.6140350877192979</v>
+      </c>
+      <c r="K48" s="3">
+        <v>10.14799154334038</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
+        <v>43861</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="4">
+      <c r="D49" s="4">
         <v>17</v>
       </c>
-      <c r="C49" s="4">
+      <c r="E49" s="4">
         <v>74</v>
       </c>
-      <c r="D49" s="4">
+      <c r="F49" s="4">
         <v>3435</v>
       </c>
-      <c r="E49" s="4">
+      <c r="G49" s="4">
         <v>947</v>
       </c>
-      <c r="F49" s="5">
+      <c r="H49" s="5">
         <v>0.18681318681318601</v>
       </c>
-      <c r="G49" s="5">
+      <c r="I49" s="5">
         <v>0.78388863532633501</v>
       </c>
+      <c r="J49" s="5">
+        <v>1.7634854771784232</v>
+      </c>
+      <c r="K49" s="5">
+        <v>3.2227488151658754</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="C1:C49" xr:uid="{211EDF4C-3C07-4D4E-AB32-18815F0AF05B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>